<commit_message>
Updated DMIs and run scripts
</commit_message>
<xml_diff>
--- a/Database/Ingest/PacifiCorp_Observations_Import.xlsx
+++ b/Database/Ingest/PacifiCorp_Observations_Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\KlamathOpsModel\Database\Ingest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E8AEDA-6E4C-412B-B489-CDAB7B14A615}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57908F49-12C8-451C-8F11-1CE51E739477}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676" xr2:uid="{415E1877-5855-4F9B-8C95-813B2C9F0A4E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676" activeTab="2" xr2:uid="{415E1877-5855-4F9B-8C95-813B2C9F0A4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Accretions Information" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Accretions.Keno to IGD Accretions PacifiCorp (cfs)</t>
-  </si>
-  <si>
     <t>Keno to IGD Accretions</t>
   </si>
   <si>
@@ -54,13 +51,16 @@
   <si>
     <t>Pulled from IGD Calculator -&gt; USBR Daily -&gt; Accretions for PacifiCorp (cfs)</t>
   </si>
+  <si>
+    <t>Agricultural Deliveries.Pacificorp Accretions (cfs)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm\/dd\/yy"/>
+    <numFmt numFmtId="164" formatCode="mm\/dd\/yy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -153,7 +153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -472,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D16CFE-F16B-4D21-B5A3-2527780AC55F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -484,18 +484,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -508,7 +508,7 @@
   <dimension ref="A1:B1980"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1647" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1683" sqref="B1683"/>
     </sheetView>
   </sheetViews>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -15478,8 +15478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE81D635-3EB7-4164-8EF7-EDE23E12270D}">
   <dimension ref="A1:B2124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15490,7 +15490,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>